<commit_message>
Commit code for separate excels
</commit_message>
<xml_diff>
--- a/HolidayReport.xlsx
+++ b/HolidayReport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Holiday date</t>
   </si>
@@ -349,26 +349,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="1"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>